<commit_message>
Refactored and QoL changes
</commit_message>
<xml_diff>
--- a/someProject/Template/Student_Details.xlsx
+++ b/someProject/Template/Student_Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\someProject\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE111FFC-14EC-4FF5-A1A4-CFC675C1AE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D15FE4B-2BC3-48A9-B884-9D0CCA08BB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2172" yWindow="3372" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>21WU0101056</t>
-  </si>
-  <si>
-    <t>Harsh Morayya</t>
-  </si>
-  <si>
-    <t>2021-2025</t>
-  </si>
-  <si>
-    <t>CSE</t>
-  </si>
-  <si>
-    <t>hars@sas.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Roll no.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Specialization</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>phone no.</t>
+  </si>
+  <si>
+    <t>Program code</t>
+  </si>
+  <si>
+    <t>&lt;Start inserting data in this row&gt;</t>
   </si>
 </sst>
 </file>
@@ -368,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,7 +391,7 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,16 +407,24 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1">
-        <v>3</v>
-      </c>
-      <c r="G1">
-        <v>9223573015</v>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" xr:uid="{D46B0632-9EFA-40C3-99CC-E4F52718CB0E}"/>
+    <hyperlink ref="E1" r:id="rId1" display="hars@sas.com" xr:uid="{D46B0632-9EFA-40C3-99CC-E4F52718CB0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>